<commit_message>
added reset sheet route
</commit_message>
<xml_diff>
--- a/Participants.xlsx
+++ b/Participants.xlsx
@@ -1,74 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4D31D9-899E-4252-BF76-EBD87D6F206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Participants" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Participants" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Имя</t>
-  </si>
-  <si>
-    <t>Номер телефона</t>
-  </si>
-  <si>
-    <t>Мессенджер</t>
-  </si>
-  <si>
-    <t>Вопрос №1</t>
-  </si>
-  <si>
-    <t>Вопрос №2</t>
-  </si>
-  <si>
-    <t>Вопрос №3</t>
-  </si>
-  <si>
-    <t>Вопрос №4</t>
-  </si>
-  <si>
-    <t>Вопрос №5</t>
-  </si>
-  <si>
-    <t>Вопрос №6</t>
-  </si>
-  <si>
-    <t>Вопрос №7</t>
-  </si>
-  <si>
-    <t>Вопрос №8</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,12 +44,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,56 +384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="11" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-  </sheetData>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>